<commit_message>
Updated application and application testing documentation
</commit_message>
<xml_diff>
--- a/CRDMA/docs/test_cases/packages/CCDP/CRDMA CCDP Test Cases.xlsx
+++ b/CRDMA/docs/test_cases/packages/CCDP/CRDMA CCDP Test Cases.xlsx
@@ -428,7 +428,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,12 +438,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,12 +454,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -473,10 +466,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,7 +750,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,54 +779,54 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="6">
         <v>-20603</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="6">
         <v>-20605</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>-20608</v>
       </c>
     </row>
@@ -867,7 +857,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,79 +886,79 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1035,7 +1025,7 @@
       <c r="E2" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>71</v>
       </c>
       <c r="G2" t="s">
@@ -1058,7 +1048,7 @@
       <c r="E3" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>73</v>
       </c>
       <c r="G3" t="s">
@@ -1081,7 +1071,7 @@
       <c r="E4" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>74</v>
       </c>
       <c r="G4" t="s">
@@ -1104,7 +1094,7 @@
       <c r="E5" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>77</v>
       </c>
       <c r="G5" t="s">
@@ -1127,7 +1117,7 @@
       <c r="E6" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>79</v>
       </c>
       <c r="G6" t="s">
@@ -1150,7 +1140,7 @@
       <c r="E7" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>81</v>
       </c>
       <c r="G7" t="s">
@@ -1173,7 +1163,7 @@
       <c r="E8" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>82</v>
       </c>
       <c r="G8" t="s">
@@ -1196,7 +1186,7 @@
       <c r="E9" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>83</v>
       </c>
       <c r="G9" t="s">
@@ -1219,7 +1209,7 @@
       <c r="E10" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>84</v>
       </c>
       <c r="G10" t="s">
@@ -1242,7 +1232,7 @@
       <c r="E11" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>85</v>
       </c>
       <c r="G11" t="s">
@@ -1265,7 +1255,7 @@
       <c r="E12" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G12" t="s">
@@ -1288,7 +1278,7 @@
       <c r="E13" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>88</v>
       </c>
       <c r="G13" t="s">
@@ -1311,7 +1301,7 @@
       <c r="E14" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>89</v>
       </c>
       <c r="G14" t="s">
@@ -1334,7 +1324,7 @@
       <c r="E15" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>90</v>
       </c>
       <c r="G15" t="s">
@@ -1357,7 +1347,7 @@
       <c r="E16" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>91</v>
       </c>
       <c r="G16" t="s">
@@ -1380,7 +1370,7 @@
       <c r="E17" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>92</v>
       </c>
       <c r="G17" t="s">
@@ -1403,7 +1393,7 @@
       <c r="E18" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>93</v>
       </c>
       <c r="G18" t="s">
@@ -1426,7 +1416,7 @@
       <c r="E19" t="s">
         <v>72</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>94</v>
       </c>
       <c r="G19" t="s">
@@ -1449,7 +1439,7 @@
       <c r="E20" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>95</v>
       </c>
       <c r="G20" t="s">
@@ -1472,7 +1462,7 @@
       <c r="E21" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>97</v>
       </c>
       <c r="G21" t="s">
@@ -1495,7 +1485,7 @@
       <c r="E22" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>98</v>
       </c>
       <c r="G22" t="s">
@@ -1518,7 +1508,7 @@
       <c r="E23" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>99</v>
       </c>
       <c r="G23" t="s">
@@ -1541,7 +1531,7 @@
       <c r="E24" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>100</v>
       </c>
       <c r="G24" t="s">
@@ -1564,7 +1554,7 @@
       <c r="E25" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>101</v>
       </c>
       <c r="G25" t="s">
@@ -1587,7 +1577,7 @@
       <c r="E26" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>102</v>
       </c>
       <c r="G26" t="s">
@@ -1610,7 +1600,7 @@
       <c r="E27" t="s">
         <v>87</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>103</v>
       </c>
       <c r="G27" t="s">
@@ -1633,7 +1623,7 @@
       <c r="E28" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>104</v>
       </c>
       <c r="G28" t="s">
@@ -1656,7 +1646,7 @@
       <c r="E29" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>105</v>
       </c>
       <c r="G29" t="s">
@@ -1679,7 +1669,7 @@
       <c r="E30" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>106</v>
       </c>
       <c r="G30" t="s">
@@ -1699,7 +1689,7 @@
       <c r="E31" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>107</v>
       </c>
       <c r="G31" t="s">
@@ -1719,7 +1709,7 @@
       <c r="E32" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>108</v>
       </c>
       <c r="G32" t="s">
@@ -1739,7 +1729,7 @@
       <c r="E33" t="s">
         <v>78</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>109</v>
       </c>
       <c r="G33" t="s">
@@ -1759,7 +1749,7 @@
       <c r="E34" t="s">
         <v>70</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>110</v>
       </c>
       <c r="G34" t="s">
@@ -1779,7 +1769,7 @@
       <c r="E35" t="s">
         <v>76</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>111</v>
       </c>
       <c r="G35" t="s">
@@ -1802,7 +1792,7 @@
       <c r="E36" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>112</v>
       </c>
       <c r="G36" t="s">
@@ -1825,7 +1815,7 @@
       <c r="E37" t="s">
         <v>72</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="4" t="s">
         <v>113</v>
       </c>
       <c r="G37" t="s">
@@ -1848,7 +1838,7 @@
       <c r="E38" t="s">
         <v>72</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G38" t="s">
@@ -1871,7 +1861,7 @@
       <c r="E39" t="s">
         <v>115</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="4" t="s">
         <v>116</v>
       </c>
       <c r="G39" t="s">
@@ -1894,7 +1884,7 @@
       <c r="E40" t="s">
         <v>115</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="4" t="s">
         <v>117</v>
       </c>
       <c r="G40" t="s">
@@ -1917,7 +1907,7 @@
       <c r="E41" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="4" t="s">
         <v>118</v>
       </c>
       <c r="G41" t="s">
@@ -1940,7 +1930,7 @@
       <c r="E42" t="s">
         <v>87</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="4" t="s">
         <v>119</v>
       </c>
       <c r="G42" t="s">
@@ -1963,7 +1953,7 @@
       <c r="E43" t="s">
         <v>87</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="4" t="s">
         <v>120</v>
       </c>
       <c r="G43" t="s">
@@ -1986,7 +1976,7 @@
       <c r="E44" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="4" t="s">
         <v>121</v>
       </c>
       <c r="G44" t="s">
@@ -2009,7 +1999,7 @@
       <c r="E45" t="s">
         <v>72</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="4" t="s">
         <v>122</v>
       </c>
       <c r="G45" t="s">
@@ -2032,7 +2022,7 @@
       <c r="E46" t="s">
         <v>72</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="4" t="s">
         <v>123</v>
       </c>
       <c r="G46" t="s">
@@ -2055,7 +2045,7 @@
       <c r="E47" t="s">
         <v>115</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="4" t="s">
         <v>124</v>
       </c>
       <c r="G47" t="s">
@@ -2078,7 +2068,7 @@
       <c r="E48" t="s">
         <v>115</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="4" t="s">
         <v>125</v>
       </c>
       <c r="G48" t="s">

</xml_diff>